<commit_message>
Valor Hominis in Sanguine Dei
</commit_message>
<xml_diff>
--- a/tools/scrapy/readings/readings/urls.xlsx
+++ b/tools/scrapy/readings/readings/urls.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
   <si>
     <t>full database</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>http://en.katabiblon.com/us/index.php?text=LXX&amp;book=2Chr&amp;ch=1</t>
+  </si>
+  <si>
+    <t>http://www.ewtn.com/daily-readings/?date=</t>
   </si>
   <si>
     <t>http://en.katabiblon.com/us/index.php?text=LXX&amp;book=1Esd&amp;ch=1</t>
@@ -278,11 +281,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -293,10 +297,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -315,26 +343,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -361,29 +374,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -391,6 +381,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -406,16 +397,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,6 +433,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -446,187 +450,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,6 +641,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -660,15 +684,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,26 +718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -737,18 +732,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -758,135 +762,137 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,13 +1207,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="12" max="12" width="11.3636363636364"/>
+    <col min="13" max="13" width="26.3636363636364" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
@@ -1247,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L11" si="1">"'"&amp;K4&amp;"',"</f>
+        <f t="shared" ref="L4:L12" si="1">"'"&amp;K4&amp;"',"</f>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=1Mc&amp;ch=1',</v>
       </c>
     </row>
@@ -1304,7 +1314,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" ref="D8:D39" si="2">"'"&amp;C8&amp;"',"</f>
+        <f t="shared" ref="D8:D40" si="2">"'"&amp;C8&amp;"',"</f>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=JgsB&amp;ch=1',</v>
       </c>
       <c r="K8" t="s">
@@ -1375,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="L12" t="str">
-        <f>"'"&amp;K12&amp;"',"</f>
+        <f t="shared" si="1"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Sir&amp;ch=1',</v>
       </c>
     </row>
@@ -1397,7 +1407,7 @@
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=1Chr&amp;ch=1',</v>
       </c>
     </row>
-    <row r="15" spans="3:4">
+    <row r="15" spans="3:13">
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -1405,35 +1415,75 @@
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=2Chr&amp;ch=1',</v>
       </c>
-    </row>
-    <row r="16" spans="3:4">
+      <c r="K15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="2">
+        <v>42728</v>
+      </c>
+      <c r="M15" t="str">
+        <f>"'"&amp;K15&amp;TEXT(L15,"yyyy-mm-dd")&amp;"',"</f>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-24',</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13">
       <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=1Esd&amp;ch=1',</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="2"/>
-        <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=1Esd&amp;ch=1',</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
+      <c r="L16" s="2">
+        <v>42729</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" ref="M16:M22" si="3">"'"&amp;K16&amp;TEXT(L16,"yyyy-mm-dd")&amp;"',"</f>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-25',</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13">
       <c r="C17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=2Esd&amp;ch=1',</v>
       </c>
-    </row>
-    <row r="18" spans="3:4">
+      <c r="K17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="2">
+        <v>42730</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="3"/>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-26',</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13">
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Est&amp;ch=1',</v>
       </c>
-    </row>
-    <row r="19" spans="3:4">
+      <c r="K18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="2">
+        <v>42731</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="3"/>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-27',</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13">
       <c r="C19" t="s">
         <v>17</v>
       </c>
@@ -1441,8 +1491,18 @@
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Jdt&amp;ch=1',</v>
       </c>
-    </row>
-    <row r="20" spans="3:4">
+      <c r="K19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="2">
+        <v>42732</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="3"/>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-28',</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13">
       <c r="C20" t="s">
         <v>15</v>
       </c>
@@ -1450,8 +1510,18 @@
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=TbBA&amp;ch=1',</v>
       </c>
-    </row>
-    <row r="21" spans="3:4">
+      <c r="K20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="2">
+        <v>42733</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="3"/>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-29',</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13">
       <c r="C21" t="s">
         <v>5</v>
       </c>
@@ -1459,14 +1529,34 @@
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=1Mc&amp;ch=1',</v>
       </c>
-    </row>
-    <row r="22" spans="3:4">
+      <c r="K21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="2">
+        <v>42734</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="3"/>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-30',</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13">
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=2Mc&amp;ch=1',</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="2">
+        <v>42735</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="3"/>
+        <v>'http://www.ewtn.com/daily-readings/?date=2016-12-31',</v>
       </c>
     </row>
     <row r="23" spans="3:4">
@@ -1489,7 +1579,7 @@
     </row>
     <row r="25" spans="3:4">
       <c r="C25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="2"/>
@@ -1498,7 +1588,7 @@
     </row>
     <row r="26" spans="3:4">
       <c r="C26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="2"/>
@@ -1507,7 +1597,7 @@
     </row>
     <row r="27" spans="3:4">
       <c r="C27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="2"/>
@@ -1516,7 +1606,7 @@
     </row>
     <row r="28" spans="3:4">
       <c r="C28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="2"/>
@@ -1525,7 +1615,7 @@
     </row>
     <row r="29" spans="3:4">
       <c r="C29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="2"/>
@@ -1534,7 +1624,7 @@
     </row>
     <row r="30" spans="3:4">
       <c r="C30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="2"/>
@@ -1555,142 +1645,142 @@
         <v>21</v>
       </c>
       <c r="D32" t="str">
-        <f>"'"&amp;C32&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Sir&amp;ch=1',</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D33" t="str">
-        <f>"'"&amp;C33&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=PsSol&amp;ch=1',</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D34" t="str">
-        <f>"'"&amp;C34&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Hos&amp;ch=1',</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D35" t="str">
-        <f>"'"&amp;C35&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Mi&amp;ch=1',</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D36" t="str">
-        <f>"'"&amp;C36&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Am&amp;ch=1',</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D37" t="str">
-        <f>"'"&amp;C37&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Jl&amp;ch=1',</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D38" t="str">
-        <f>"'"&amp;C38&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Jon&amp;ch=1',</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D39" t="str">
-        <f>"'"&amp;C39&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Ob&amp;ch=1',</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D40" t="str">
-        <f>"'"&amp;C40&amp;"',"</f>
+        <f t="shared" si="2"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Na&amp;ch=1',</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D85" si="3">"'"&amp;C41&amp;"',"</f>
+        <f t="shared" ref="D41:D85" si="4">"'"&amp;C41&amp;"',"</f>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Hb&amp;ch=1',</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Zep&amp;ch=1',</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Hg&amp;ch=1',</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Zec&amp;ch=1',</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Mal&amp;ch=1',</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Is&amp;ch=1',</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Jer&amp;ch=1',</v>
       </c>
     </row>
@@ -1699,347 +1789,357 @@
         <v>13</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Bar&amp;ch=1',</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=EpJer&amp;ch=1',</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Lam&amp;ch=1',</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=Ez&amp;ch=1',</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=DnOG&amp;ch=1',</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=DnTh&amp;ch=1',</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=SusOG&amp;ch=1',</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=SusTh&amp;ch=1',</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=BelOG&amp;ch=1',</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=LXX&amp;book=BelTh&amp;ch=1',</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Mt&amp;ch=1',</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Mk&amp;ch=1',</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Lk&amp;ch=1',</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Jn&amp;ch=1',</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Acts&amp;ch=1',</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Rom&amp;ch=1',</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=1Cor&amp;ch=1',</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=2Cor&amp;ch=1',</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Gal&amp;ch=1',</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Gal&amp;ch=1',</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Eph&amp;ch=1',</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Phil&amp;ch=1',</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Col&amp;ch=1',</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=1Thes&amp;ch=1',</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=2Thes&amp;ch=1',</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=1Tm&amp;ch=1',</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=2Tm&amp;ch=1',</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Ti&amp;ch=1',</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Phlm&amp;ch=1',</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Heb&amp;ch=1',</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Jas&amp;ch=1',</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=1Pt&amp;ch=1',</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=2Pt&amp;ch=1',</v>
       </c>
     </row>
     <row r="81" spans="3:4">
       <c r="C81" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=1Jn&amp;ch=1',</v>
       </c>
     </row>
     <row r="82" spans="3:4">
       <c r="C82" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=2Jn&amp;ch=1',</v>
       </c>
     </row>
     <row r="83" spans="3:4">
       <c r="C83" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=3Jn&amp;ch=1',</v>
       </c>
     </row>
     <row r="84" spans="3:4">
       <c r="C84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Jude&amp;ch=1',</v>
       </c>
     </row>
     <row r="85" spans="3:4">
       <c r="C85" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>'http://en.katabiblon.com/us/index.php?text=GNT&amp;book=Rv&amp;ch=1',</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K15" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K16" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K17" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K18" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K19" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K20" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K21" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+    <hyperlink ref="K22" r:id="rId1" display="http://www.ewtn.com/daily-readings/?date="/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>